<commit_message>
E1: Classes, métodos, atributos, objeto, herança e formulários
</commit_message>
<xml_diff>
--- a/Tarefa3/Teste_mesa_fracoes.xlsx
+++ b/Tarefa3/Teste_mesa_fracoes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/35e95fd1eb072d23/Área de Trabalho/FATEC/2º SEM/Laboratório de Desenvolvimento em Banco de Dados/LPI/Tarefa3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA9D8FF0-1634-4C27-BA54-74E5C223D07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{EA9D8FF0-1634-4C27-BA54-74E5C223D07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABB273D0-F834-4926-BFDC-86E1D46FED7A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9600B9F2-3ACF-4CEC-8CAF-BB88A0C561BF}"/>
+    <workbookView xWindow="11700" yWindow="192" windowWidth="10908" windowHeight="8880" xr2:uid="{9600B9F2-3ACF-4CEC-8CAF-BB88A0C561BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -100,13 +100,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -446,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27151FD5-59FE-491F-A056-59E3A99BD840}">
   <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,15 +455,16 @@
     <col min="4" max="5" width="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" customWidth="1"/>
+    <col min="10" max="10" width="3.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="2">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2">
@@ -474,7 +473,7 @@
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="3">
         <f>(B3*D2)+(B2*D3)</f>
         <v>23</v>
       </c>
@@ -489,25 +488,25 @@
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <f>B3*D3</f>
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <f>(B5*D6)-(B6*D5)</f>
         <v>22</v>
       </c>
@@ -519,35 +518,35 @@
       <c r="D6">
         <v>7</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="4">
         <f>B6*D6</f>
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="4">
+      <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <v>2</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="2">
         <v>3</v>
       </c>
       <c r="G8" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="2">
         <f>(B8*D9)+(B9*D8)</f>
         <v>26</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="3">
         <f>(H8*F9)+(H9*F8)</f>
         <v>97</v>
       </c>
@@ -569,29 +568,29 @@
         <f>B9*D9</f>
         <v>15</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="4">
         <f>F9*H9</f>
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="4">
+      <c r="B11" s="2">
         <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="2">
         <v>4</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="2">
         <f>(B11*D12)-(B12*D11)</f>
         <v>18</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="3">
         <f>F11/9</f>
         <v>2</v>
       </c>
@@ -607,35 +606,35 @@
         <f>B12*D12</f>
         <v>9</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <f>F12/9</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="4">
+      <c r="B14" s="2">
         <v>2</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="2">
         <v>1</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="2">
         <v>5</v>
       </c>
       <c r="G14" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="2">
         <f>(B14*D15)+(B15*D14)</f>
         <v>7</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="3">
         <f>(H14*F15)-(H15*F14)</f>
         <v>13</v>
       </c>
@@ -654,41 +653,41 @@
         <f>B15*D15</f>
         <v>3</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="4">
         <f>H15*F15</f>
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="4">
+      <c r="B17" s="2">
         <v>5</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="2">
         <v>4</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="2">
         <v>2</v>
       </c>
       <c r="G17" t="s">
         <v>0</v>
       </c>
-      <c r="H17" s="4">
-        <f>(D17*F18)-(D18*F17)</f>
-        <v>14</v>
-      </c>
-      <c r="I17" s="4">
-        <f>B17*H17</f>
-        <v>70</v>
-      </c>
-      <c r="J17" s="5">
-        <f>I17/10</f>
-        <v>7</v>
+      <c r="H17" s="2">
+        <f>(B17*D17)</f>
+        <v>20</v>
+      </c>
+      <c r="I17" s="2">
+        <f>(H17*F18)-(H18*F17)</f>
+        <v>88</v>
+      </c>
+      <c r="J17" s="3">
+        <f>I17/2</f>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
@@ -702,32 +701,32 @@
         <v>5</v>
       </c>
       <c r="H18">
-        <f>D18*F18</f>
+        <f>B18*D18</f>
+        <v>6</v>
+      </c>
+      <c r="I18">
+        <f>H18*F18</f>
+        <v>30</v>
+      </c>
+      <c r="J18" s="4">
+        <f>I18/2</f>
         <v>15</v>
       </c>
-      <c r="I18">
-        <f>B18*H18</f>
-        <v>30</v>
-      </c>
-      <c r="J18" s="6">
-        <f>I18/10</f>
-        <v>3</v>
-      </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="4">
+      <c r="B20" s="2">
         <v>5</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="2">
         <v>2</v>
       </c>
       <c r="E20" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="3">
         <f>(B20*D21)+(B21*D20)</f>
         <v>37</v>
       </c>
@@ -739,25 +738,25 @@
       <c r="D21">
         <v>7</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="4">
         <f>B21*D21</f>
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="4">
+      <c r="B23" s="2">
         <v>5</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="2">
         <v>7</v>
       </c>
       <c r="E23" t="s">
         <v>0</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="3">
         <f>B23*D23</f>
         <v>35</v>
       </c>
@@ -769,7 +768,7 @@
       <c r="D24">
         <v>4</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="4">
         <f>B24*D24</f>
         <v>12</v>
       </c>

</xml_diff>